<commit_message>
finalized flask quiz for 'Intro to Flask' backlog item and updated flask routes excel file
</commit_message>
<xml_diff>
--- a/project_journal/assets/s7_assets/initial_flask_routes.xlsx
+++ b/project_journal/assets/s7_assets/initial_flask_routes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grego\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grego\Desktop\Coding\Projects\plan_tool\project_journal\assets\s7_assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677DEFBB-16DC-4D81-A333-D24C78935637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE1B0911-A0DB-445E-815B-A6D2C5B1B736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C551EE5F-BC6E-4444-BA40-FE73DEA46AED}"/>
   </bookViews>

</xml_diff>